<commit_message>
CE01ISSP Cal and Ingest files
removed m from depth on cal sheets, commented out NUTNR and OPTAA on
ingest CSV ( data is not telemetered), deleted templates.
</commit_message>
<xml_diff>
--- a/CE01ISSP/Omaha_Cal_Info_CE01ISSP_00001.xlsx
+++ b/CE01ISSP/Omaha_Cal_Info_CE01ISSP_00001.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="600" windowWidth="25600" windowHeight="16060" tabRatio="579" activeTab="1"/>
+    <workbookView xWindow="1005" yWindow="600" windowWidth="25605" windowHeight="16065" tabRatio="579" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Asset_Cal_Info!$A$1:$G$51</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="102">
   <si>
     <t>Ref Des</t>
   </si>
@@ -242,9 +242,6 @@
     <t>Constant.  wlupper = Upper wavelength limit for spectra fit. From DPS: 240 nm (1-cm pathlength probe tip) or 245 nm (4-cm pathlength probe tip)</t>
   </si>
   <si>
-    <t>25 m</t>
-  </si>
-  <si>
     <t>Requires TEMPWAT, PRESWAT and PRACSAL from CE06ISSP-SP001-09-CTDPFJ000</t>
   </si>
   <si>
@@ -359,10 +356,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="167" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="36" x14ac:knownFonts="1">
     <font>
@@ -598,6 +595,7 @@
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -711,14 +709,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
@@ -1230,7 +1228,7 @@
     <xf numFmtId="14" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1249,10 +1247,10 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1321,7 +1319,7 @@
     <xf numFmtId="11" fontId="25" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="25" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="25" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="20" fontId="25" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="25" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1853,7 +1851,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Read Me"/>
@@ -2194,27 +2192,27 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" customWidth="1"/>
-    <col min="11" max="11" width="18.33203125" customWidth="1"/>
-    <col min="12" max="12" width="15.1640625" customWidth="1"/>
-    <col min="13" max="13" width="13.83203125" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="6" customFormat="1" ht="28">
+    <row r="1" spans="1:13" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2249,12 +2247,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="42" t="s">
         <v>92</v>
-      </c>
-      <c r="B2" s="42" t="s">
-        <v>93</v>
       </c>
       <c r="C2" s="42">
         <v>1</v>
@@ -2272,8 +2270,8 @@
       <c r="H2" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="I2" s="43" t="s">
-        <v>70</v>
+      <c r="I2" s="43">
+        <v>25</v>
       </c>
       <c r="J2" s="43" t="s">
         <v>37</v>
@@ -2287,91 +2285,91 @@
         <v>-124.09816666666667</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="9" customFormat="1">
+    <row r="3" spans="1:13" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C3" s="10"/>
       <c r="D3" s="11"/>
       <c r="E3" s="12"/>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:13" s="9" customFormat="1">
+    <row r="4" spans="1:13" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C4" s="10"/>
       <c r="D4" s="11"/>
       <c r="E4" s="12"/>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:13" s="9" customFormat="1">
+    <row r="5" spans="1:13" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C5" s="10"/>
       <c r="D5" s="11"/>
       <c r="E5" s="12"/>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:13" s="9" customFormat="1">
+    <row r="6" spans="1:13" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C6" s="10"/>
       <c r="D6" s="11"/>
       <c r="E6" s="12"/>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:13" s="9" customFormat="1">
+    <row r="7" spans="1:13" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C7" s="10"/>
       <c r="D7" s="11"/>
       <c r="E7" s="12"/>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" spans="1:13" s="9" customFormat="1">
+    <row r="8" spans="1:13" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C8" s="10"/>
       <c r="D8" s="11"/>
       <c r="E8" s="12"/>
       <c r="F8" s="11"/>
     </row>
-    <row r="9" spans="1:13" s="9" customFormat="1">
+    <row r="9" spans="1:13" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C9" s="10"/>
       <c r="D9" s="11"/>
       <c r="E9" s="12"/>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" spans="1:13" s="9" customFormat="1">
+    <row r="10" spans="1:13" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C10" s="10"/>
       <c r="D10" s="11"/>
       <c r="E10" s="12"/>
       <c r="F10" s="11"/>
     </row>
-    <row r="11" spans="1:13" s="9" customFormat="1">
+    <row r="11" spans="1:13" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C11" s="10"/>
       <c r="D11" s="11"/>
       <c r="E11" s="12"/>
       <c r="F11" s="11"/>
     </row>
-    <row r="12" spans="1:13" s="9" customFormat="1">
+    <row r="12" spans="1:13" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C12" s="10"/>
       <c r="D12" s="11"/>
       <c r="E12" s="12"/>
       <c r="F12" s="11"/>
     </row>
-    <row r="13" spans="1:13" s="9" customFormat="1">
+    <row r="13" spans="1:13" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C13" s="10"/>
       <c r="D13" s="11"/>
       <c r="E13" s="12"/>
       <c r="F13" s="11"/>
     </row>
-    <row r="14" spans="1:13" s="9" customFormat="1">
+    <row r="14" spans="1:13" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C14" s="10"/>
       <c r="D14" s="11"/>
       <c r="E14" s="12"/>
       <c r="F14" s="11"/>
     </row>
-    <row r="15" spans="1:13" s="9" customFormat="1">
+    <row r="15" spans="1:13" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C15" s="10"/>
       <c r="D15" s="11"/>
       <c r="E15" s="12"/>
       <c r="F15" s="11"/>
     </row>
-    <row r="16" spans="1:13" s="9" customFormat="1">
+    <row r="16" spans="1:13" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
       <c r="E16" s="12"/>
       <c r="F16" s="11"/>
     </row>
-    <row r="17" spans="3:6" s="9" customFormat="1">
+    <row r="17" spans="3:6" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C17" s="10"/>
       <c r="D17" s="11"/>
       <c r="E17" s="12"/>
@@ -2399,18 +2397,18 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="4" width="17" style="7" customWidth="1"/>
-    <col min="5" max="5" width="37.83203125" customWidth="1"/>
-    <col min="6" max="6" width="57.33203125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="21.33203125" customWidth="1"/>
+    <col min="5" max="5" width="37.85546875" customWidth="1"/>
+    <col min="6" max="6" width="57.28515625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28">
+    <row r="1" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -2433,7 +2431,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="19"/>
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
@@ -2442,12 +2440,12 @@
       <c r="F2" s="20"/>
       <c r="G2" s="21"/>
     </row>
-    <row r="3" spans="1:7" s="7" customFormat="1">
+    <row r="3" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C3" s="24">
         <v>1</v>
@@ -2465,12 +2463,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="7" customFormat="1">
+    <row r="4" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C4" s="28">
         <v>1</v>
@@ -2488,12 +2486,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="7" customFormat="1" ht="15">
+    <row r="5" spans="1:7" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" s="28">
         <v>1</v>
@@ -2508,15 +2506,15 @@
         <v>11</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="7" customFormat="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6" s="28">
         <v>1</v>
@@ -2525,16 +2523,16 @@
         <v>209</v>
       </c>
       <c r="E6" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="G6" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="F6" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="G6" s="24" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="7" customFormat="1">
+    </row>
+    <row r="7" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
       <c r="B7" s="27"/>
       <c r="C7" s="28"/>
@@ -2543,12 +2541,12 @@
       <c r="F7" s="25"/>
       <c r="G7" s="20"/>
     </row>
-    <row r="8" spans="1:7" s="7" customFormat="1">
+    <row r="8" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C8" s="24">
         <v>1</v>
@@ -2560,18 +2558,18 @@
         <v>56</v>
       </c>
       <c r="F8" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G8" s="30" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="7" customFormat="1">
+    <row r="9" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C9" s="28">
         <v>1</v>
@@ -2583,16 +2581,16 @@
         <v>58</v>
       </c>
       <c r="F9" s="41" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G9" s="31"/>
     </row>
-    <row r="10" spans="1:7" s="7" customFormat="1">
+    <row r="10" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C10" s="28">
         <v>1</v>
@@ -2608,12 +2606,12 @@
       </c>
       <c r="G10" s="31"/>
     </row>
-    <row r="11" spans="1:7" s="7" customFormat="1">
+    <row r="11" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C11" s="28">
         <v>1</v>
@@ -2625,16 +2623,16 @@
         <v>57</v>
       </c>
       <c r="F11" s="41" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G11" s="31"/>
     </row>
-    <row r="12" spans="1:7" s="7" customFormat="1">
+    <row r="12" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C12" s="28">
         <v>1</v>
@@ -2646,16 +2644,16 @@
         <v>52</v>
       </c>
       <c r="F12" s="41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G12" s="31"/>
     </row>
-    <row r="13" spans="1:7" s="7" customFormat="1">
+    <row r="13" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C13" s="28">
         <v>1</v>
@@ -2667,16 +2665,16 @@
         <v>53</v>
       </c>
       <c r="F13" s="41" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G13" s="31"/>
     </row>
-    <row r="14" spans="1:7" s="7" customFormat="1">
+    <row r="14" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C14" s="28">
         <v>1</v>
@@ -2688,16 +2686,16 @@
         <v>55</v>
       </c>
       <c r="F14" s="41" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G14" s="31"/>
     </row>
-    <row r="15" spans="1:7" s="7" customFormat="1">
+    <row r="15" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C15" s="28">
         <v>1</v>
@@ -2709,11 +2707,11 @@
         <v>59</v>
       </c>
       <c r="F15" s="41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G15" s="31"/>
     </row>
-    <row r="16" spans="1:7" s="7" customFormat="1">
+    <row r="16" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
       <c r="B16" s="27"/>
       <c r="C16" s="28"/>
@@ -2722,12 +2720,12 @@
       <c r="F16" s="25"/>
       <c r="G16" s="20"/>
     </row>
-    <row r="17" spans="1:7" s="7" customFormat="1">
+    <row r="17" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C17" s="24">
         <v>1</v>
@@ -2745,12 +2743,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="7" customFormat="1">
+    <row r="18" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C18" s="28">
         <v>1</v>
@@ -2768,7 +2766,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="7" customFormat="1">
+    <row r="19" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
       <c r="B19" s="27"/>
       <c r="C19" s="28"/>
@@ -2777,12 +2775,12 @@
       <c r="F19" s="25"/>
       <c r="G19" s="20"/>
     </row>
-    <row r="20" spans="1:7" s="7" customFormat="1">
+    <row r="20" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C20" s="24">
         <v>1</v>
@@ -2800,12 +2798,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="7" customFormat="1">
+    <row r="21" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C21" s="28">
         <v>1</v>
@@ -2823,12 +2821,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="7" customFormat="1">
+    <row r="22" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C22" s="28">
         <v>1</v>
@@ -2846,12 +2844,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="7" customFormat="1">
+    <row r="23" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C23" s="28">
         <v>1</v>
@@ -2863,18 +2861,18 @@
         <v>45</v>
       </c>
       <c r="F23" s="42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G23" s="20" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="7" customFormat="1">
+    <row r="24" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C24" s="28">
         <v>1</v>
@@ -2886,18 +2884,18 @@
         <v>47</v>
       </c>
       <c r="F24" s="42" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G24" s="20" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="7" customFormat="1">
+    <row r="25" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C25" s="28">
         <v>1</v>
@@ -2909,18 +2907,18 @@
         <v>49</v>
       </c>
       <c r="F25" s="42" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G25" s="20" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="7" customFormat="1">
+    <row r="26" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C26" s="28">
         <v>1</v>
@@ -2932,13 +2930,13 @@
         <v>51</v>
       </c>
       <c r="F26" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="G26" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="G26" s="20" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" s="7" customFormat="1">
+    </row>
+    <row r="27" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
       <c r="B27" s="27"/>
       <c r="C27" s="28"/>
@@ -2947,12 +2945,12 @@
       <c r="F27" s="25"/>
       <c r="G27" s="20"/>
     </row>
-    <row r="28" spans="1:7" s="7" customFormat="1">
+    <row r="28" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C28" s="24">
         <v>1</v>
@@ -2964,16 +2962,16 @@
         <v>38</v>
       </c>
       <c r="F28" s="43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G28" s="20"/>
     </row>
-    <row r="29" spans="1:7" s="7" customFormat="1">
+    <row r="29" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C29" s="28">
         <v>1</v>
@@ -2985,16 +2983,16 @@
         <v>39</v>
       </c>
       <c r="F29" s="43" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G29" s="20"/>
     </row>
-    <row r="30" spans="1:7" s="7" customFormat="1">
+    <row r="30" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B30" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C30" s="28">
         <v>1</v>
@@ -3006,11 +3004,11 @@
         <v>40</v>
       </c>
       <c r="F30" s="43" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G30" s="20"/>
     </row>
-    <row r="31" spans="1:7" s="7" customFormat="1">
+    <row r="31" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="22"/>
       <c r="B31" s="27"/>
       <c r="C31" s="28"/>
@@ -3019,12 +3017,12 @@
       <c r="F31" s="25"/>
       <c r="G31" s="20"/>
     </row>
-    <row r="32" spans="1:7" s="7" customFormat="1">
+    <row r="32" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C32" s="24">
         <v>1</v>
@@ -3042,12 +3040,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="7" customFormat="1">
+    <row r="33" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B33" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C33" s="28">
         <v>1</v>
@@ -3065,12 +3063,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="7" customFormat="1">
+    <row r="34" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B34" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C34" s="28">
         <v>1</v>
@@ -3088,12 +3086,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="7" customFormat="1">
+    <row r="35" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B35" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C35" s="28">
         <v>1</v>
@@ -3111,12 +3109,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="7" customFormat="1">
+    <row r="36" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C36" s="28">
         <v>1</v>
@@ -3134,12 +3132,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="7" customFormat="1">
+    <row r="37" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B37" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C37" s="28">
         <v>1</v>
@@ -3157,12 +3155,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="7" customFormat="1">
+    <row r="38" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C38" s="28">
         <v>1</v>
@@ -3180,12 +3178,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="7" customFormat="1">
+    <row r="39" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B39" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C39" s="28">
         <v>1</v>
@@ -3203,12 +3201,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="7" customFormat="1">
+    <row r="40" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B40" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C40" s="28">
         <v>1</v>
@@ -3226,12 +3224,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:7" s="7" customFormat="1">
+    <row r="41" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B41" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C41" s="28">
         <v>1</v>
@@ -3249,7 +3247,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="7" customFormat="1">
+    <row r="42" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="26"/>
       <c r="B42" s="27"/>
       <c r="C42" s="28"/>
@@ -3258,18 +3256,18 @@
       <c r="F42" s="25"/>
       <c r="G42" s="20"/>
     </row>
-    <row r="43" spans="1:7" s="7" customFormat="1">
+    <row r="43" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B43" s="23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C43" s="24">
         <v>1</v>
       </c>
       <c r="D43" s="37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E43" s="20" t="s">
         <v>9</v>
@@ -3281,18 +3279,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="7" customFormat="1">
+    <row r="44" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B44" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C44" s="28">
         <v>1</v>
       </c>
       <c r="D44" s="37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E44" s="20" t="s">
         <v>10</v>
@@ -3304,7 +3302,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:7" s="7" customFormat="1">
+    <row r="45" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="22"/>
       <c r="B45" s="27"/>
       <c r="C45" s="28"/>
@@ -3313,12 +3311,12 @@
       <c r="F45" s="25"/>
       <c r="G45" s="20"/>
     </row>
-    <row r="46" spans="1:7" s="7" customFormat="1">
+    <row r="46" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B46" s="23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C46" s="24">
         <v>1</v>
@@ -3334,12 +3332,12 @@
       </c>
       <c r="G46" s="20"/>
     </row>
-    <row r="47" spans="1:7" s="7" customFormat="1">
+    <row r="47" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B47" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C47" s="28">
         <v>1</v>
@@ -3355,12 +3353,12 @@
       </c>
       <c r="G47" s="20"/>
     </row>
-    <row r="48" spans="1:7" s="7" customFormat="1">
+    <row r="48" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B48" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C48" s="28">
         <v>1</v>
@@ -3376,7 +3374,7 @@
       </c>
       <c r="G48" s="20"/>
     </row>
-    <row r="49" spans="1:7" s="13" customFormat="1">
+    <row r="49" spans="1:7" s="13" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A49" s="33"/>
       <c r="B49" s="33"/>
       <c r="C49" s="24"/>
@@ -3385,27 +3383,27 @@
       <c r="F49" s="34"/>
       <c r="G49" s="33"/>
     </row>
-    <row r="50" spans="1:7" s="7" customFormat="1">
+    <row r="50" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="35" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B50" s="23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C50" s="24">
         <v>1</v>
       </c>
       <c r="D50" s="39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E50" s="20"/>
       <c r="F50" s="36"/>
       <c r="G50" s="20"/>
     </row>
-    <row r="51" spans="1:7" s="7" customFormat="1"/>
-    <row r="52" spans="1:7" s="7" customFormat="1"/>
-    <row r="53" spans="1:7" s="7" customFormat="1"/>
-    <row r="54" spans="1:7" s="7" customFormat="1"/>
+    <row r="51" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="34" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3426,9 +3424,9 @@
       <selection sqref="A1:AJ85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>4.6008E-2</v>
       </c>
@@ -3538,7 +3536,7 @@
         <v>-1.137E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:36">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4.2536999999999998E-2</v>
       </c>
@@ -3648,7 +3646,7 @@
         <v>-1.358E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:36">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4.3115000000000001E-2</v>
       </c>
@@ -3758,7 +3756,7 @@
         <v>-1.5838999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:36">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4.3878E-2</v>
       </c>
@@ -3868,7 +3866,7 @@
         <v>-1.8959E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:36">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4.3221000000000002E-2</v>
       </c>
@@ -3978,7 +3976,7 @@
         <v>-2.0358000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:36">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4.1510999999999999E-2</v>
       </c>
@@ -4088,7 +4086,7 @@
         <v>-1.9682000000000002E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:36">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3.7416999999999999E-2</v>
       </c>
@@ -4198,7 +4196,7 @@
         <v>-1.8426000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:36">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3.4866000000000001E-2</v>
       </c>
@@ -4308,7 +4306,7 @@
         <v>-1.6534E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:36">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3.1199999999999999E-2</v>
       </c>
@@ -4418,7 +4416,7 @@
         <v>-1.4978999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:36">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2.7692999999999999E-2</v>
       </c>
@@ -4528,7 +4526,7 @@
         <v>-1.3599999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:36">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2.4787E-2</v>
       </c>
@@ -4638,7 +4636,7 @@
         <v>-1.2409E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:36">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2.1585E-2</v>
       </c>
@@ -4748,7 +4746,7 @@
         <v>-1.1106E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:36">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1.9362999999999998E-2</v>
       </c>
@@ -4858,7 +4856,7 @@
         <v>-1.0659999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:36">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1.7412E-2</v>
       </c>
@@ -4968,7 +4966,7 @@
         <v>-1.0090999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:36">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1.5740000000000001E-2</v>
       </c>
@@ -5078,7 +5076,7 @@
         <v>-9.4520000000000003E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:36">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1.4527E-2</v>
       </c>
@@ -5188,7 +5186,7 @@
         <v>-9.214E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:36">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1.379E-2</v>
       </c>
@@ -5298,7 +5296,7 @@
         <v>-9.1629999999999993E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:36">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1.2543E-2</v>
       </c>
@@ -5408,7 +5406,7 @@
         <v>-9.1640000000000003E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:36">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1.1979999999999999E-2</v>
       </c>
@@ -5518,7 +5516,7 @@
         <v>-9.2560000000000003E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:36">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1.141E-2</v>
       </c>
@@ -5628,7 +5626,7 @@
         <v>-9.3310000000000008E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:36">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1.0869999999999999E-2</v>
       </c>
@@ -5738,7 +5736,7 @@
         <v>-9.4339999999999997E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:36">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1.0403000000000001E-2</v>
       </c>
@@ -5848,7 +5846,7 @@
         <v>-9.6699999999999998E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:36">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1.018E-2</v>
       </c>
@@ -5958,7 +5956,7 @@
         <v>-9.9600000000000001E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:36">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>9.5879999999999993E-3</v>
       </c>
@@ -6068,7 +6066,7 @@
         <v>-9.9190000000000007E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:36">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>9.384E-3</v>
       </c>
@@ -6178,7 +6176,7 @@
         <v>-1.0031999999999999E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:36">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>9.025E-3</v>
       </c>
@@ -6288,7 +6286,7 @@
         <v>-9.8969999999999995E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:36">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>8.5540000000000008E-3</v>
       </c>
@@ -6398,7 +6396,7 @@
         <v>-9.5949999999999994E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:36">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>8.3199999999999993E-3</v>
       </c>
@@ -6508,7 +6506,7 @@
         <v>-9.2449999999999997E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:36">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>7.9459999999999999E-3</v>
       </c>
@@ -6618,7 +6616,7 @@
         <v>-8.9110000000000005E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:36">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>7.5760000000000003E-3</v>
       </c>
@@ -6728,7 +6726,7 @@
         <v>-8.286E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:36">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>7.5640000000000004E-3</v>
       </c>
@@ -6838,7 +6836,7 @@
         <v>-7.8480000000000008E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:36">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>7.2570000000000004E-3</v>
       </c>
@@ -6948,7 +6946,7 @@
         <v>-7.273E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:36">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>7.1209999999999997E-3</v>
       </c>
@@ -7058,7 +7056,7 @@
         <v>-6.6730000000000001E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:36">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>7.1009999999999997E-3</v>
       </c>
@@ -7168,7 +7166,7 @@
         <v>-6.0819999999999997E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:36">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>6.9690000000000004E-3</v>
       </c>
@@ -7278,7 +7276,7 @@
         <v>-5.555E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:36">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>7.1580000000000003E-3</v>
       </c>
@@ -7388,7 +7386,7 @@
         <v>-5.0730000000000003E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:36">
+    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>7.0470000000000003E-3</v>
       </c>
@@ -7498,7 +7496,7 @@
         <v>-4.6169999999999996E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:36">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>7.2830000000000004E-3</v>
       </c>
@@ -7608,7 +7606,7 @@
         <v>-4.3220000000000003E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:36">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>7.0229999999999997E-3</v>
       </c>
@@ -7718,7 +7716,7 @@
         <v>-4.0289999999999996E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:36">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>6.6090000000000003E-3</v>
       </c>
@@ -7828,7 +7826,7 @@
         <v>-3.7910000000000001E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:36">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>6.4440000000000001E-3</v>
       </c>
@@ -7938,7 +7936,7 @@
         <v>-3.5990000000000002E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:36">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>5.9170000000000004E-3</v>
       </c>
@@ -8048,7 +8046,7 @@
         <v>-3.4169999999999999E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:36">
+    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1.9090000000000001E-3</v>
       </c>
@@ -8158,7 +8156,7 @@
         <v>-4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:36">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1.421E-3</v>
       </c>
@@ -8268,7 +8266,7 @@
         <v>-1.9699999999999999E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:36">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1.3699999999999999E-3</v>
       </c>
@@ -8378,7 +8376,7 @@
         <v>6.6000000000000005E-5</v>
       </c>
     </row>
-    <row r="46" spans="1:36">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>9.7599999999999998E-4</v>
       </c>
@@ -8488,7 +8486,7 @@
         <v>3.4499999999999998E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:36">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>5.5900000000000004E-4</v>
       </c>
@@ -8598,7 +8596,7 @@
         <v>6.4800000000000003E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:36">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>-1.1E-5</v>
       </c>
@@ -8708,7 +8706,7 @@
         <v>1.0020000000000001E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:36">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>-5.62E-4</v>
       </c>
@@ -8818,7 +8816,7 @@
         <v>1.3500000000000001E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:36">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>-1.3389999999999999E-3</v>
       </c>
@@ -8928,7 +8926,7 @@
         <v>1.5380000000000001E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:36">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>-2.0699999999999998E-3</v>
       </c>
@@ -9038,7 +9036,7 @@
         <v>1.722E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:36">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>-2.702E-3</v>
       </c>
@@ -9148,7 +9146,7 @@
         <v>1.714E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:36">
+    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>-2.8639999999999998E-3</v>
       </c>
@@ -9258,7 +9256,7 @@
         <v>1.7279999999999999E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:36">
+    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>-2.9510000000000001E-3</v>
       </c>
@@ -9368,7 +9366,7 @@
         <v>1.5299999999999999E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:36">
+    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>-2.8219999999999999E-3</v>
       </c>
@@ -9478,7 +9476,7 @@
         <v>1.3780000000000001E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:36">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>-2.7550000000000001E-3</v>
       </c>
@@ -9588,7 +9586,7 @@
         <v>1.0640000000000001E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:36">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>-2.5140000000000002E-3</v>
       </c>
@@ -9698,7 +9696,7 @@
         <v>9.3599999999999998E-4</v>
       </c>
     </row>
-    <row r="58" spans="1:36">
+    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>-2.2439999999999999E-3</v>
       </c>
@@ -9808,7 +9806,7 @@
         <v>8.25E-4</v>
       </c>
     </row>
-    <row r="59" spans="1:36">
+    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>-2.0070000000000001E-3</v>
       </c>
@@ -9918,7 +9916,7 @@
         <v>6.9899999999999997E-4</v>
       </c>
     </row>
-    <row r="60" spans="1:36">
+    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>-1.7780000000000001E-3</v>
       </c>
@@ -10028,7 +10026,7 @@
         <v>6.3199999999999997E-4</v>
       </c>
     </row>
-    <row r="61" spans="1:36">
+    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>-1.655E-3</v>
       </c>
@@ -10138,7 +10136,7 @@
         <v>4.6700000000000002E-4</v>
       </c>
     </row>
-    <row r="62" spans="1:36">
+    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>-1.6310000000000001E-3</v>
       </c>
@@ -10248,7 +10246,7 @@
         <v>3.2499999999999999E-4</v>
       </c>
     </row>
-    <row r="63" spans="1:36">
+    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>-1.5989999999999999E-3</v>
       </c>
@@ -10358,7 +10356,7 @@
         <v>1.93E-4</v>
       </c>
     </row>
-    <row r="64" spans="1:36">
+    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>-1.493E-3</v>
       </c>
@@ -10468,7 +10466,7 @@
         <v>6.4999999999999994E-5</v>
       </c>
     </row>
-    <row r="65" spans="1:36">
+    <row r="65" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>-1.273E-3</v>
       </c>
@@ -10578,7 +10576,7 @@
         <v>-7.4999999999999993E-5</v>
       </c>
     </row>
-    <row r="66" spans="1:36">
+    <row r="66" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>-1.0189999999999999E-3</v>
       </c>
@@ -10688,7 +10686,7 @@
         <v>-1.5899999999999999E-4</v>
       </c>
     </row>
-    <row r="67" spans="1:36">
+    <row r="67" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>-7.1699999999999997E-4</v>
       </c>
@@ -10798,7 +10796,7 @@
         <v>-1.7000000000000001E-4</v>
       </c>
     </row>
-    <row r="68" spans="1:36">
+    <row r="68" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>-1.8E-5</v>
       </c>
@@ -10908,7 +10906,7 @@
         <v>-3.1100000000000002E-4</v>
       </c>
     </row>
-    <row r="69" spans="1:36">
+    <row r="69" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>3.28E-4</v>
       </c>
@@ -11018,7 +11016,7 @@
         <v>-5.0299999999999997E-4</v>
       </c>
     </row>
-    <row r="70" spans="1:36">
+    <row r="70" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>5.8299999999999997E-4</v>
       </c>
@@ -11128,7 +11126,7 @@
         <v>-6.7100000000000005E-4</v>
       </c>
     </row>
-    <row r="71" spans="1:36">
+    <row r="71" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>8.4999999999999995E-4</v>
       </c>
@@ -11238,7 +11236,7 @@
         <v>-9.0499999999999999E-4</v>
       </c>
     </row>
-    <row r="72" spans="1:36">
+    <row r="72" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>1.165E-3</v>
       </c>
@@ -11348,7 +11346,7 @@
         <v>-1.168E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:36">
+    <row r="73" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>1.469E-3</v>
       </c>
@@ -11458,7 +11456,7 @@
         <v>-1.3760000000000001E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:36">
+    <row r="74" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>1.9949999999999998E-3</v>
       </c>
@@ -11568,7 +11566,7 @@
         <v>-1.586E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:36">
+    <row r="75" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2.3739999999999998E-3</v>
       </c>
@@ -11678,7 +11676,7 @@
         <v>-1.663E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:36">
+    <row r="76" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2.3760000000000001E-3</v>
       </c>
@@ -11788,7 +11786,7 @@
         <v>-1.732E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:36">
+    <row r="77" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2.4130000000000002E-3</v>
       </c>
@@ -11898,7 +11896,7 @@
         <v>-1.681E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:36">
+    <row r="78" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2.166E-3</v>
       </c>
@@ -12008,7 +12006,7 @@
         <v>-1.699E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:36">
+    <row r="79" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>1.9530000000000001E-3</v>
       </c>
@@ -12118,7 +12116,7 @@
         <v>-1.627E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:36">
+    <row r="80" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>1.7539999999999999E-3</v>
       </c>
@@ -12228,7 +12226,7 @@
         <v>-1.565E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:36">
+    <row r="81" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>1.653E-3</v>
       </c>
@@ -12338,7 +12336,7 @@
         <v>-1.4779999999999999E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:36">
+    <row r="82" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>1.4339999999999999E-3</v>
       </c>
@@ -12448,7 +12446,7 @@
         <v>-1.253E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:36">
+    <row r="83" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>1.5529999999999999E-3</v>
       </c>
@@ -12558,7 +12556,7 @@
         <v>-1.103E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:36">
+    <row r="84" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>1.704E-3</v>
       </c>
@@ -12668,7 +12666,7 @@
         <v>-8.92E-4</v>
       </c>
     </row>
-    <row r="85" spans="1:36">
+    <row r="85" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>1.725E-3</v>
       </c>
@@ -12796,9 +12794,9 @@
       <selection activeCell="O106" sqref="O106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0.11464299999999999</v>
       </c>
@@ -12908,7 +12906,7 @@
         <v>-5.0855999999999998E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:36">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.11143699999999999</v>
       </c>
@@ -13018,7 +13016,7 @@
         <v>-4.8311E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:36">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.10566</v>
       </c>
@@ -13128,7 +13126,7 @@
         <v>-4.7612000000000002E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:36">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.103315</v>
       </c>
@@ -13238,7 +13236,7 @@
         <v>-4.4401000000000003E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:36">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.100078</v>
       </c>
@@ -13348,7 +13346,7 @@
         <v>-4.3917999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:36">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>9.7517999999999994E-2</v>
       </c>
@@ -13458,7 +13456,7 @@
         <v>-4.0932999999999997E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:36">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>9.4977000000000006E-2</v>
       </c>
@@ -13568,7 +13566,7 @@
         <v>-3.9729E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:36">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>9.2086000000000001E-2</v>
       </c>
@@ -13678,7 +13676,7 @@
         <v>-3.8157999999999997E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:36">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8.8232000000000005E-2</v>
       </c>
@@ -13788,7 +13786,7 @@
         <v>-3.6015999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:36">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8.4955000000000003E-2</v>
       </c>
@@ -13898,7 +13896,7 @@
         <v>-3.3876000000000003E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:36">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8.2607E-2</v>
       </c>
@@ -14008,7 +14006,7 @@
         <v>-3.2259999999999997E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:36">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>7.9913999999999999E-2</v>
       </c>
@@ -14118,7 +14116,7 @@
         <v>-3.0206E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:36">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>7.8973000000000002E-2</v>
       </c>
@@ -14228,7 +14226,7 @@
         <v>-2.8332E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:36">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>7.6024999999999995E-2</v>
       </c>
@@ -14338,7 +14336,7 @@
         <v>-2.6426000000000002E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:36">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>7.4902999999999997E-2</v>
       </c>
@@ -14448,7 +14446,7 @@
         <v>-2.4596E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:36">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>7.3431999999999997E-2</v>
       </c>
@@ -14558,7 +14556,7 @@
         <v>-2.2771E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:36">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>7.2954000000000005E-2</v>
       </c>
@@ -14668,7 +14666,7 @@
         <v>-2.1378000000000001E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:36">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>7.2392999999999999E-2</v>
       </c>
@@ -14778,7 +14776,7 @@
         <v>-2.0163E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:36">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>7.1642999999999998E-2</v>
       </c>
@@ -14888,7 +14886,7 @@
         <v>-1.9016999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:36">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>7.0186999999999999E-2</v>
       </c>
@@ -14998,7 +14996,7 @@
         <v>-1.8008E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:36">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>6.9302000000000002E-2</v>
       </c>
@@ -15108,7 +15106,7 @@
         <v>-1.7052000000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:36">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>6.8472000000000005E-2</v>
       </c>
@@ -15218,7 +15216,7 @@
         <v>-1.6406E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:36">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>6.7325999999999997E-2</v>
       </c>
@@ -15328,7 +15326,7 @@
         <v>-1.5685000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:36">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>6.6239999999999993E-2</v>
       </c>
@@ -15438,7 +15436,7 @@
         <v>-1.5491E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:36">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>6.5568000000000001E-2</v>
       </c>
@@ -15548,7 +15546,7 @@
         <v>-1.5266999999999999E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:36">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>6.4459000000000002E-2</v>
       </c>
@@ -15658,7 +15656,7 @@
         <v>-1.5446E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:36">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>6.3698000000000005E-2</v>
       </c>
@@ -15768,7 +15766,7 @@
         <v>-1.5762000000000002E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:36">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>6.2205000000000003E-2</v>
       </c>
@@ -15878,7 +15876,7 @@
         <v>-1.5906E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:36">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>6.1772000000000001E-2</v>
       </c>
@@ -15988,7 +15986,7 @@
         <v>-1.6376000000000002E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:36">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>6.0983000000000002E-2</v>
       </c>
@@ -16098,7 +16096,7 @@
         <v>-1.6698000000000001E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:36">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>5.9484000000000002E-2</v>
       </c>
@@ -16208,7 +16206,7 @@
         <v>-1.7065E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:36">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>5.885E-2</v>
       </c>
@@ -16318,7 +16316,7 @@
         <v>-1.7538000000000002E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:36">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>5.8035000000000003E-2</v>
       </c>
@@ -16428,7 +16426,7 @@
         <v>-1.7956E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:36">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>5.6728000000000001E-2</v>
       </c>
@@ -16538,7 +16536,7 @@
         <v>-1.8258E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:36">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>5.6006E-2</v>
       </c>
@@ -16648,7 +16646,7 @@
         <v>-1.8557000000000001E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:36">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>5.4544000000000002E-2</v>
       </c>
@@ -16758,7 +16756,7 @@
         <v>-1.8412999999999999E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:36">
+    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>5.3428000000000003E-2</v>
       </c>
@@ -16868,7 +16866,7 @@
         <v>-1.8096000000000001E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:36">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>5.2255000000000003E-2</v>
       </c>
@@ -16978,7 +16976,7 @@
         <v>-1.7731E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:36">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>5.1347999999999998E-2</v>
       </c>
@@ -17088,7 +17086,7 @@
         <v>-1.7405E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:36">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>5.0941E-2</v>
       </c>
@@ -17198,7 +17196,7 @@
         <v>-1.6965000000000001E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:36">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>5.0456000000000001E-2</v>
       </c>
@@ -17308,7 +17306,7 @@
         <v>-1.6688000000000001E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:36">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>4.9521000000000003E-2</v>
       </c>
@@ -17418,7 +17416,7 @@
         <v>-1.6479000000000001E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:36">
+    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>5.2349E-2</v>
       </c>
@@ -17528,7 +17526,7 @@
         <v>-1.9583E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:36">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>5.2712000000000002E-2</v>
       </c>
@@ -17638,7 +17636,7 @@
         <v>-1.9982E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:36">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>5.2965999999999999E-2</v>
       </c>
@@ -17748,7 +17746,7 @@
         <v>-2.0264000000000001E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:36">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>5.373E-2</v>
       </c>
@@ -17858,7 +17856,7 @@
         <v>-2.0386000000000001E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:36">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>5.4421999999999998E-2</v>
       </c>
@@ -17968,7 +17966,7 @@
         <v>-2.0745E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:36">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>5.5028000000000001E-2</v>
       </c>
@@ -18078,7 +18076,7 @@
         <v>-2.0560999999999999E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:36">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>5.5216000000000001E-2</v>
       </c>
@@ -18188,7 +18186,7 @@
         <v>-2.0379999999999999E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:36">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>5.5146000000000001E-2</v>
       </c>
@@ -18298,7 +18296,7 @@
         <v>-1.9935000000000001E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:36">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>5.4336000000000002E-2</v>
       </c>
@@ -18408,7 +18406,7 @@
         <v>-1.9289000000000001E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:36">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>5.3359999999999998E-2</v>
       </c>
@@ -18518,7 +18516,7 @@
         <v>-1.8554999999999999E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:36">
+    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>5.2211E-2</v>
       </c>
@@ -18628,7 +18626,7 @@
         <v>-1.8151E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:36">
+    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>5.0758999999999999E-2</v>
       </c>
@@ -18738,7 +18736,7 @@
         <v>-1.7795999999999999E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:36">
+    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>4.9699E-2</v>
       </c>
@@ -18848,7 +18846,7 @@
         <v>-1.7281000000000001E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:36">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>4.9028000000000002E-2</v>
       </c>
@@ -18958,7 +18956,7 @@
         <v>-1.6966999999999999E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:36">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>4.8057000000000002E-2</v>
       </c>
@@ -19068,7 +19066,7 @@
         <v>-1.6674999999999999E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:36">
+    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>4.7393999999999999E-2</v>
       </c>
@@ -19178,7 +19176,7 @@
         <v>-1.6372000000000001E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:36">
+    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>4.6948999999999998E-2</v>
       </c>
@@ -19288,7 +19286,7 @@
         <v>-1.6211E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:36">
+    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>4.6358000000000003E-2</v>
       </c>
@@ -19398,7 +19396,7 @@
         <v>-1.5982E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:36">
+    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>4.6005999999999998E-2</v>
       </c>
@@ -19508,7 +19506,7 @@
         <v>-1.5730999999999998E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:36">
+    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>4.5657000000000003E-2</v>
       </c>
@@ -19618,7 +19616,7 @@
         <v>-1.5650000000000001E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:36">
+    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>4.4887999999999997E-2</v>
       </c>
@@ -19728,7 +19726,7 @@
         <v>-1.5442000000000001E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:36">
+    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>4.4344000000000001E-2</v>
       </c>
@@ -19838,7 +19836,7 @@
         <v>-1.5474999999999999E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:36">
+    <row r="65" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>4.3698000000000001E-2</v>
       </c>
@@ -19948,7 +19946,7 @@
         <v>-1.5446E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:36">
+    <row r="66" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>4.2992000000000002E-2</v>
       </c>
@@ -20058,7 +20056,7 @@
         <v>-1.5382E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:36">
+    <row r="67" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>4.2221000000000002E-2</v>
       </c>
@@ -20168,7 +20166,7 @@
         <v>-1.5272000000000001E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:36">
+    <row r="68" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>4.2258999999999998E-2</v>
       </c>
@@ -20278,7 +20276,7 @@
         <v>-1.5022000000000001E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:36">
+    <row r="69" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>4.1813000000000003E-2</v>
       </c>
@@ -20388,7 +20386,7 @@
         <v>-1.4598E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:36">
+    <row r="70" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>4.1190999999999998E-2</v>
       </c>
@@ -20498,7 +20496,7 @@
         <v>-1.439E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:36">
+    <row r="71" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>4.1315999999999999E-2</v>
       </c>
@@ -20608,7 +20606,7 @@
         <v>-1.4239E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:36">
+    <row r="72" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>4.0593999999999998E-2</v>
       </c>
@@ -20718,7 +20716,7 @@
         <v>-1.4161E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:36">
+    <row r="73" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>4.0902000000000001E-2</v>
       </c>
@@ -20828,7 +20826,7 @@
         <v>-1.4272999999999999E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:36">
+    <row r="74" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>4.0507000000000001E-2</v>
       </c>
@@ -20938,7 +20936,7 @@
         <v>-1.4279999999999999E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:36">
+    <row r="75" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>4.1043999999999997E-2</v>
       </c>
@@ -21048,7 +21046,7 @@
         <v>-1.4352999999999999E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:36">
+    <row r="76" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>4.0555000000000001E-2</v>
       </c>
@@ -21158,7 +21156,7 @@
         <v>-1.4429000000000001E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:36">
+    <row r="77" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>4.1255E-2</v>
       </c>
@@ -21268,7 +21266,7 @@
         <v>-1.4637000000000001E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:36">
+    <row r="78" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>4.0912999999999998E-2</v>
       </c>
@@ -21378,7 +21376,7 @@
         <v>-1.4713E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:36">
+    <row r="79" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>4.1392999999999999E-2</v>
       </c>
@@ -21488,7 +21486,7 @@
         <v>-1.5044E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:36">
+    <row r="80" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>4.0951000000000001E-2</v>
       </c>
@@ -21598,7 +21596,7 @@
         <v>-1.5200999999999999E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:36">
+    <row r="81" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>4.0934999999999999E-2</v>
       </c>
@@ -21708,7 +21706,7 @@
         <v>-1.54E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:36">
+    <row r="82" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>4.0092999999999997E-2</v>
       </c>
@@ -21818,7 +21816,7 @@
         <v>-1.5492000000000001E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:36">
+    <row r="83" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>3.9625E-2</v>
       </c>
@@ -21928,7 +21926,7 @@
         <v>-1.5389E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:36">
+    <row r="84" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>3.8066000000000003E-2</v>
       </c>
@@ -22038,7 +22036,7 @@
         <v>-1.4987E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:36">
+    <row r="85" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>3.8646E-2</v>
       </c>

</xml_diff>